<commit_message>
removed PrEP_CT.R, PrEP_CT.T_1, PrEP_CT.T, PrEP_CT.TestResult.T
- removed PrEP_CT.R, PrEP_CT.T_1, PrEP_CT.T, PrEP_CT.TestResult.T
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/25Tto26TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/25Tto26TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF96C39-7A17-1146-9411-E2C3ABB37845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617C0524-591E-554D-86BC-A70A9C8F49E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="49300" yWindow="760" windowWidth="34700" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Map" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Map!$A$1:$N$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Map!$A$1:$N$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="183">
   <si>
     <t>CXCA_SCRN</t>
   </si>
@@ -485,9 +485,6 @@
     <t>OVC_SERV.Grad.T</t>
   </si>
   <si>
-    <t>PrEP_CT.T</t>
-  </si>
-  <si>
     <t>PrEP_CT.KP.T</t>
   </si>
   <si>
@@ -516,9 +513,6 @@
   </si>
   <si>
     <t>fy24_age_bands</t>
-  </si>
-  <si>
-    <t>PrEP_CT.TestResult.T</t>
   </si>
   <si>
     <t>HTS.Index.Pos.T</t>
@@ -1475,11 +1469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1549,7 +1543,7 @@
         <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1570,7 +1564,7 @@
         <v>83</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>2</v>
@@ -1593,7 +1587,7 @@
         <v>107</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1614,7 +1608,7 @@
         <v>83</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>2</v>
@@ -1637,7 +1631,7 @@
         <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1658,10 +1652,10 @@
         <v>75</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>37</v>
@@ -1681,7 +1675,7 @@
         <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -1702,10 +1696,10 @@
         <v>104</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>41</v>
@@ -1725,7 +1719,7 @@
         <v>112</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -1746,10 +1740,10 @@
         <v>104</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>41</v>
@@ -1769,7 +1763,7 @@
         <v>113</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -1790,10 +1784,10 @@
         <v>82</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>37</v>
@@ -1813,7 +1807,7 @@
         <v>114</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -1834,10 +1828,10 @@
         <v>82</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>37</v>
@@ -1857,7 +1851,7 @@
         <v>115</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -1878,7 +1872,7 @@
         <v>80</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>2</v>
@@ -1901,7 +1895,7 @@
         <v>116</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -1922,7 +1916,7 @@
         <v>80</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>2</v>
@@ -1945,7 +1939,7 @@
         <v>117</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -1966,7 +1960,7 @@
         <v>78</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>2</v>
@@ -1989,7 +1983,7 @@
         <v>118</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -2010,7 +2004,7 @@
         <v>79</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>2</v>
@@ -2033,7 +2027,7 @@
         <v>119</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>9</v>
@@ -2054,7 +2048,7 @@
         <v>78</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>2</v>
@@ -2077,7 +2071,7 @@
         <v>120</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -2098,7 +2092,7 @@
         <v>81</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>2</v>
@@ -2121,7 +2115,7 @@
         <v>121</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>12</v>
@@ -2136,16 +2130,16 @@
         <v>57</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>37</v>
@@ -2165,7 +2159,7 @@
         <v>149</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
@@ -2180,16 +2174,16 @@
         <v>57</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>37</v>
@@ -2209,7 +2203,7 @@
         <v>148</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>12</v>
@@ -2224,16 +2218,16 @@
         <v>57</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>37</v>
@@ -2253,7 +2247,7 @@
         <v>122</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>13</v>
@@ -2274,10 +2268,10 @@
         <v>92</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>41</v>
@@ -2297,7 +2291,7 @@
         <v>123</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>13</v>
@@ -2318,10 +2312,10 @@
         <v>92</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>41</v>
@@ -2341,7 +2335,7 @@
         <v>124</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
@@ -2362,10 +2356,10 @@
         <v>75</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>41</v>
@@ -2385,7 +2379,7 @@
         <v>125</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>14</v>
@@ -2406,10 +2400,10 @@
         <v>77</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>41</v>
@@ -2429,7 +2423,7 @@
         <v>126</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>14</v>
@@ -2450,10 +2444,10 @@
         <v>77</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>41</v>
@@ -2473,7 +2467,7 @@
         <v>127</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>14</v>
@@ -2494,10 +2488,10 @@
         <v>77</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>41</v>
@@ -2517,13 +2511,13 @@
         <v>150</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>29</v>
@@ -2532,22 +2526,22 @@
         <v>57</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>160</v>
+        <v>2</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>2</v>
@@ -2558,16 +2552,16 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>170</v>
+        <v>170</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>29</v>
@@ -2576,22 +2570,22 @@
         <v>57</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>2</v>
+        <v>159</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>2</v>
@@ -2602,10 +2596,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>17</v>
@@ -2620,22 +2614,22 @@
         <v>57</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>160</v>
+        <v>2</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>2</v>
@@ -2646,43 +2640,43 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>39</v>
@@ -2690,10 +2684,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>18</v>
@@ -2714,7 +2708,7 @@
         <v>92</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>86</v>
@@ -2726,18 +2720,18 @@
         <v>2</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>18</v>
@@ -2746,10 +2740,10 @@
         <v>67</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>91</v>
@@ -2758,7 +2752,7 @@
         <v>92</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>86</v>
@@ -2770,18 +2764,18 @@
         <v>2</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>18</v>
@@ -2802,7 +2796,7 @@
         <v>92</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>86</v>
@@ -2814,7 +2808,7 @@
         <v>2</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>39</v>
@@ -2822,16 +2816,16 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>29</v>
@@ -2839,17 +2833,17 @@
       <c r="F31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>92</v>
+      <c r="G31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>37</v>
@@ -2858,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>39</v>
@@ -2866,16 +2860,16 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>29</v>
@@ -2884,16 +2878,16 @@
         <v>57</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>37</v>
@@ -2902,7 +2896,7 @@
         <v>2</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>39</v>
@@ -2910,16 +2904,16 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>29</v>
@@ -2934,10 +2928,10 @@
         <v>76</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>37</v>
@@ -2954,10 +2948,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>21</v>
@@ -2972,22 +2966,22 @@
         <v>57</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>160</v>
+        <v>2</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>2</v>
@@ -2998,16 +2992,16 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>29</v>
@@ -3022,7 +3016,7 @@
         <v>79</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>2</v>
@@ -3042,22 +3036,22 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>69</v>
+        <v>170</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>22</v>
@@ -3066,7 +3060,7 @@
         <v>79</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>2</v>
@@ -3086,10 +3080,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>23</v>
@@ -3098,10 +3092,10 @@
         <v>71</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>22</v>
@@ -3110,7 +3104,7 @@
         <v>79</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>2</v>
@@ -3130,10 +3124,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>23</v>
@@ -3142,31 +3136,31 @@
         <v>71</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>2</v>
+        <v>159</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>2</v>
+        <v>172</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>39</v>
@@ -3174,10 +3168,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>23</v>
@@ -3186,10 +3180,10 @@
         <v>71</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>24</v>
@@ -3198,10 +3192,10 @@
         <v>93</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>37</v>
@@ -3210,7 +3204,7 @@
         <v>2</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>39</v>
@@ -3218,34 +3212,34 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>71</v>
+        <v>170</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>37</v>
@@ -3254,7 +3248,7 @@
         <v>2</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>174</v>
+        <v>98</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>39</v>
@@ -3262,10 +3256,10 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>25</v>
@@ -3286,7 +3280,7 @@
         <v>97</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>86</v>
@@ -3298,7 +3292,7 @@
         <v>2</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N41" s="2" t="s">
         <v>39</v>
@@ -3306,10 +3300,10 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>25</v>
@@ -3330,7 +3324,7 @@
         <v>97</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>86</v>
@@ -3342,7 +3336,7 @@
         <v>2</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N42" s="2" t="s">
         <v>39</v>
@@ -3350,10 +3344,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>25</v>
@@ -3374,7 +3368,7 @@
         <v>97</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J43" s="6" t="s">
         <v>86</v>
@@ -3386,7 +3380,7 @@
         <v>2</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N43" s="2" t="s">
         <v>39</v>
@@ -3394,43 +3388,43 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>39</v>
@@ -3438,16 +3432,16 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>27</v>
+        <v>170</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>29</v>
@@ -3462,36 +3456,36 @@
         <v>76</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N45" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>146</v>
+      <c r="A46" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>29</v>
@@ -3499,17 +3493,17 @@
       <c r="F46" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>76</v>
+      <c r="G46" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>41</v>
@@ -3526,16 +3520,16 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>12</v>
+        <v>170</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>29</v>
@@ -3543,28 +3537,28 @@
       <c r="F47" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>155</v>
+      <c r="G47" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M47" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N47" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N47" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3573,31 +3567,31 @@
         <v>161</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E48" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>75</v>
+        <v>176</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>37</v>
@@ -3606,7 +3600,7 @@
         <v>2</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>39</v>
@@ -3617,13 +3611,13 @@
         <v>162</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>29</v>
@@ -3632,16 +3626,16 @@
         <v>57</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>37</v>
@@ -3649,8 +3643,8 @@
       <c r="L49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M49" s="3" t="s">
-        <v>50</v>
+      <c r="M49" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>39</v>
@@ -3661,13 +3655,13 @@
         <v>163</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>29</v>
@@ -3676,16 +3670,16 @@
         <v>57</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>37</v>
@@ -3694,7 +3688,7 @@
         <v>2</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>39</v>
@@ -3705,7 +3699,7 @@
         <v>164</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>7</v>
@@ -3720,16 +3714,16 @@
         <v>57</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>37</v>
@@ -3749,7 +3743,7 @@
         <v>165</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>7</v>
@@ -3764,16 +3758,16 @@
         <v>57</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>37</v>
@@ -3788,18 +3782,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>166</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>60</v>
+        <v>5</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>29</v>
@@ -3807,17 +3801,17 @@
       <c r="F53" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>180</v>
+      <c r="G53" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>37</v>
@@ -3834,10 +3828,10 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>7</v>
@@ -3858,10 +3852,10 @@
         <v>180</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>37</v>
@@ -3870,24 +3864,24 @@
         <v>2</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>168</v>
+        <v>109</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>147</v>
+        <v>7</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>29</v>
@@ -3895,17 +3889,17 @@
       <c r="F55" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G55" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>76</v>
+      <c r="G55" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>37</v>
@@ -3914,104 +3908,16 @@
         <v>2</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N55" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N56" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N57" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:N57" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N46">
-    <sortCondition ref="A2:A46"/>
+  <autoFilter ref="A1:N55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N45">
+    <sortCondition ref="A2:A45"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>